<commit_message>
Charts of every customer created as a seperate file with unique name and saved
</commit_message>
<xml_diff>
--- a/Database/newLoan.xlsx
+++ b/Database/newLoan.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" activeCellId="1" sqref="D10 D9"/>
@@ -599,6 +599,1713 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>divesh</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>jain</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>lkdjf</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ksjd</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>kldjf</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>lkdjsf</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>lkdjs</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>10.12.2019</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>12333</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>sdkjf</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>skdlfj</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>lkskjf</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>tn-12-c-1234</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>skdl.sdf,s,s,,s,</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>6817ce00-d6ac-11e9-a30c-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>divesh20</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>nav</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5775</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>dslfkj</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>lkjsdflkjsdf</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>lkjsdfl</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>jslkjf</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>lkjsflkj</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>14.09.2019</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>kp</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>sk</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>lkjsd</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>tn-02-v-4444</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>skjd,sdf,sd</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>83281576-d6b2-11e9-bfac-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>12.3.2019</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>as</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>tn-00-c-3</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>10.8.2019</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>tn-0-c-2</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>166c3634-d6b3-11e9-9db4-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>divesh</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">navaratan </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>9884523855</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>muth u street</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nilesh</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>navartan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>9043926651</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>muthu street</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>19.08.2019</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>120000</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>kp</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>yamaha</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>y3</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>tn-01-c-1111</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2.3</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>rc,aadhar,ration</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>bd28ec38-d6b3-11e9-92af-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>10.9.2019</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>ef4cdc68-d6b3-11e9-adde-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>9.7.1999</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>mu</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>642d5dbe-d6b4-11e9-9cff-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>10.9.2000</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>1000000</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>90ebf2e4-d6b4-11e9-b897-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>10.9.1908</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2.9</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>b229db9e-d6b4-11e9-b9df-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>10.9.2019</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>f0011f92-d6b4-11e9-b395-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>10.9.2019</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>4dc9e876-d6b5-11e9-9494-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1.1.2019</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>120000</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>b58042dc-d6b5-11e9-96b8-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>10.10.2019</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>f45ed148-d6b5-11e9-a1c5-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>10.10.2019</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>30c90b5e-d6b6-11e9-95e5-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>divesh</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>navaratan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>9884523855</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>muthu street chennai</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nilesh</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">navaratan </t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>9043926651</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>muthu street chennai</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>19.08.2019</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>120000</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>kp</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>yamaha</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>y3</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>tn-02-c-8055</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>3.4</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>x,y,z</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>b002d934-d6b6-11e9-bf69-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>divesh</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>navaratan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>9884523855</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>muthu street chennai</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>nilesh</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>navaratan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>9043926651</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>muthu street chennai</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>10.09.2019</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>kp</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>yamaha</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>y3</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>tn-02-8055</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2.6</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>aadhar</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>983</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>f237508c-d6b6-11e9-acd7-107d1a2a80c2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>